<commit_message>
openpyxl 엑셀 자료 commit v1
</commit_message>
<xml_diff>
--- a/파이썬의도구들/CH3_파이썬의도구들_라이브러리/5_openpyxl/파이썬수료증리스트.xlsx
+++ b/파이썬의도구들/CH3_파이썬의도구들_라이브러리/5_openpyxl/파이썬수료증리스트.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thate\PycharmProjects\python_tools\파이썬의도구들\CH3_파이썬의도구들_라이브러리\5_openpyxl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF442135-4B88-4C6E-88A7-22523CD3A042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F48B8-F5BF-4323-9876-E3976791DEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>홍길동</t>
   </si>
@@ -49,42 +49,6 @@
   </si>
   <si>
     <t>임하늘</t>
-  </si>
-  <si>
-    <t>윤재원</t>
-  </si>
-  <si>
-    <t>오세훈</t>
-  </si>
-  <si>
-    <t>한지민</t>
-  </si>
-  <si>
-    <t>남상민</t>
-  </si>
-  <si>
-    <t>서아름</t>
-  </si>
-  <si>
-    <t>배수현</t>
-  </si>
-  <si>
-    <t>조민재</t>
-  </si>
-  <si>
-    <t>이서윤</t>
-  </si>
-  <si>
-    <t>김하늘</t>
-  </si>
-  <si>
-    <t>박지민</t>
-  </si>
-  <si>
-    <t>최유진</t>
-  </si>
-  <si>
-    <t>정민호</t>
   </si>
   <si>
     <t>name</t>
@@ -429,243 +393,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C23"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>21</v>
+      <c r="A3">
+        <v>210100</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>210100</v>
+        <v>210101</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>210101</v>
+        <v>210102</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>210102</v>
+        <v>210103</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>210103</v>
+        <v>210104</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>210104</v>
+        <v>210105</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>210105</v>
+        <v>210106</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>210106</v>
+        <v>210107</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>210107</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>210108</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>210109</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>210110</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>210111</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>210112</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>210113</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>210114</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>210115</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>210116</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>210117</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>210118</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>210119</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>